<commit_message>
Upload Jobsheet 8 & UTS PWL
</commit_message>
<xml_diff>
--- a/public/template_kategori.xlsx
+++ b/public/template_kategori.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76F5A231-898A-4C59-9D91-5CEF8E08451B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715980D6-C0F8-4052-AE9B-5D5B3C59FE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="12" windowWidth="23004" windowHeight="12948" xr2:uid="{B42900F9-E201-43D6-8616-D33012348E8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>kode kategori</t>
   </si>
@@ -42,16 +42,10 @@
     <t>nama kategori</t>
   </si>
   <si>
-    <t>PRM</t>
+    <t>PRB</t>
   </si>
   <si>
-    <t>Peralatan Mandi</t>
-  </si>
-  <si>
-    <t>PMK</t>
-  </si>
-  <si>
-    <t>Peralatan Makan</t>
+    <t>Peralatan Bersih-bersih</t>
   </si>
 </sst>
 </file>
@@ -403,16 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E9E031-10F9-4E7D-BAF4-F7EA23740317}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -431,14 +425,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>